<commit_message>
Updated questionnaire model to allow for 2500 character labels
</commit_message>
<xml_diff>
--- a/cadasta/questionnaires/tests/files/xls-form.xlsx
+++ b/cadasta/questionnaires/tests/files/xls-form.xlsx
@@ -43,8 +43,19 @@
     <t>intro</t>
   </si>
   <si>
-    <t>This form showcases the different question types available in XLSForm. 
-The hints explain how these question types were created.</t>
+    <t>Este formulário é utilizado para capturar informação sobre os encontros com a comunidade durante o processo de delimitação.
+Estes encontros podem ser com a comunidade em geral, com a liderança, ou com povoados dentro da comunidade.  Podiam ser também seminários ao nível do posto administrativo ou distrito.
+O formulário devia ser preenchido cada vez que haja um encontro.
+Os encontros podem envolver actividades de:
+- divulgação das legislações
+- palestras, sessões de vídeo, etc.
+- sensibilização sobre o processo de delimitação da área comunitária
+- sensibilização sobre a criação da associação comunitária
+- escolha de representantes da associação 
+- encontros no ambito do DRP (historial da comunidade, organização social, etc)
+- encontros para confirmar os limites ou encontros de devolução
+O técnico pode usar o formulário para gravar informação sobre a data e lugar do encontro, o numero de participantes e os temas abordados.  Pode também gravar nomes e detalhes pessoais de representantes.
+Por favor deslizar para a frente para continuar.</t>
   </si>
   <si>
     <t>begin group</t>
@@ -372,7 +383,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -393,6 +404,11 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="4">
@@ -415,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -447,6 +463,79 @@
       </right>
       <top style="thin">
         <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -495,7 +584,7 @@
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
@@ -514,34 +603,52 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1769,7 +1876,7 @@
       <c r="B1" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="C1" t="s" s="5">
+      <c r="C1" t="s" s="6">
         <v>4</v>
       </c>
       <c r="D1" t="s" s="5">
@@ -1780,451 +1887,451 @@
       </c>
     </row>
     <row r="2" ht="27" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" t="s" s="9">
         <v>9</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" t="s" s="9">
+      <c r="A4" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="10">
+      <c r="B4" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C4" t="s" s="15">
         <v>12</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" t="s" s="13">
+      <c r="A5" t="s" s="18">
         <v>13</v>
       </c>
-      <c r="B5" t="s" s="13">
+      <c r="B5" t="s" s="18">
         <v>14</v>
       </c>
-      <c r="C5" t="s" s="13">
+      <c r="C5" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="D5" t="s" s="13">
+      <c r="D5" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" t="s" s="6">
+      <c r="A6" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" ht="8.25" customHeight="1">
-      <c r="A8" t="s" s="9">
+      <c r="A8" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B8" t="s" s="10">
+      <c r="B8" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="C8" t="s" s="10">
+      <c r="C8" t="s" s="15">
         <v>19</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" ht="51" customHeight="1">
-      <c r="A9" t="s" s="13">
+      <c r="A9" t="s" s="18">
         <v>20</v>
       </c>
-      <c r="B9" t="s" s="13">
+      <c r="B9" t="s" s="18">
         <v>21</v>
       </c>
-      <c r="C9" t="s" s="13">
+      <c r="C9" t="s" s="18">
         <v>22</v>
       </c>
-      <c r="D9" t="s" s="13">
+      <c r="D9" t="s" s="18">
         <v>23</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
-      <c r="A10" t="s" s="6">
+      <c r="A10" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="B10" t="s" s="6">
+      <c r="B10" t="s" s="7">
         <v>25</v>
       </c>
-      <c r="C10" t="s" s="6">
+      <c r="C10" t="s" s="7">
         <v>26</v>
       </c>
-      <c r="D10" t="s" s="6">
+      <c r="D10" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" ht="16.5" customHeight="1">
-      <c r="A11" t="s" s="6">
+      <c r="A11" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" ht="16.5" customHeight="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" t="s" s="9">
+      <c r="A13" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B13" t="s" s="10">
+      <c r="B13" t="s" s="15">
         <v>28</v>
       </c>
-      <c r="C13" t="s" s="10">
+      <c r="C13" t="s" s="15">
         <v>29</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" ht="51" customHeight="1">
-      <c r="A14" t="s" s="13">
+      <c r="A14" t="s" s="18">
         <v>30</v>
       </c>
-      <c r="B14" t="s" s="13">
+      <c r="B14" t="s" s="18">
         <v>31</v>
       </c>
-      <c r="C14" t="s" s="13">
+      <c r="C14" t="s" s="18">
         <v>32</v>
       </c>
-      <c r="D14" t="s" s="13">
+      <c r="D14" t="s" s="18">
         <v>33</v>
       </c>
-      <c r="E14" s="14"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" t="s" s="6">
+      <c r="A15" t="s" s="7">
         <v>34</v>
       </c>
-      <c r="B15" t="s" s="6">
+      <c r="B15" t="s" s="7">
         <v>35</v>
       </c>
-      <c r="C15" t="s" s="6">
+      <c r="C15" t="s" s="7">
         <v>36</v>
       </c>
-      <c r="D15" t="s" s="6">
+      <c r="D15" t="s" s="7">
         <v>37</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" ht="25.5" customHeight="1">
-      <c r="A16" t="s" s="6">
+      <c r="A16" t="s" s="7">
         <v>38</v>
       </c>
-      <c r="B16" t="s" s="6">
+      <c r="B16" t="s" s="7">
         <v>38</v>
       </c>
-      <c r="C16" t="s" s="6">
+      <c r="C16" t="s" s="7">
         <v>39</v>
       </c>
-      <c r="D16" t="s" s="6">
+      <c r="D16" t="s" s="7">
         <v>40</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="6">
+      <c r="A17" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" t="s" s="9">
+      <c r="A19" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B19" t="s" s="10">
+      <c r="B19" t="s" s="15">
         <v>41</v>
       </c>
-      <c r="C19" t="s" s="10">
+      <c r="C19" t="s" s="15">
         <v>42</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" ht="76.5" customHeight="1">
-      <c r="A20" t="s" s="13">
+      <c r="A20" t="s" s="18">
         <v>43</v>
       </c>
-      <c r="B20" t="s" s="13">
+      <c r="B20" t="s" s="18">
         <v>44</v>
       </c>
-      <c r="C20" t="s" s="13">
+      <c r="C20" t="s" s="18">
         <v>45</v>
       </c>
-      <c r="D20" t="s" s="13">
+      <c r="D20" t="s" s="18">
         <v>46</v>
       </c>
-      <c r="E20" s="14"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" ht="25.5" customHeight="1">
-      <c r="A21" t="s" s="6">
+      <c r="A21" t="s" s="7">
         <v>47</v>
       </c>
-      <c r="B21" t="s" s="6">
+      <c r="B21" t="s" s="7">
         <v>48</v>
       </c>
-      <c r="C21" t="s" s="6">
+      <c r="C21" t="s" s="7">
         <v>49</v>
       </c>
-      <c r="D21" t="s" s="6">
+      <c r="D21" t="s" s="7">
         <v>50</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" t="s" s="6">
+      <c r="A22" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
     </row>
     <row r="24" ht="15" customHeight="1">
-      <c r="A24" t="s" s="9">
+      <c r="A24" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B24" t="s" s="10">
+      <c r="B24" t="s" s="15">
         <v>51</v>
       </c>
-      <c r="C24" t="s" s="10">
+      <c r="C24" t="s" s="15">
         <v>52</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" ht="15" customHeight="1">
-      <c r="A25" t="s" s="13">
+      <c r="A25" t="s" s="18">
         <v>51</v>
       </c>
-      <c r="B25" t="s" s="13">
+      <c r="B25" t="s" s="18">
         <v>53</v>
       </c>
-      <c r="C25" t="s" s="13">
+      <c r="C25" t="s" s="18">
         <v>54</v>
       </c>
-      <c r="D25" t="s" s="13">
+      <c r="D25" t="s" s="18">
         <v>55</v>
       </c>
-      <c r="E25" s="14"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" t="s" s="6">
+      <c r="A26" t="s" s="7">
         <v>56</v>
       </c>
-      <c r="B26" t="s" s="6">
+      <c r="B26" t="s" s="7">
         <v>57</v>
       </c>
-      <c r="C26" t="s" s="6">
+      <c r="C26" t="s" s="7">
         <v>58</v>
       </c>
-      <c r="D26" t="s" s="6">
+      <c r="D26" t="s" s="7">
         <v>59</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" t="s" s="6">
+      <c r="A27" t="s" s="7">
         <v>60</v>
       </c>
-      <c r="B27" t="s" s="6">
+      <c r="B27" t="s" s="7">
         <v>61</v>
       </c>
-      <c r="C27" t="s" s="6">
+      <c r="C27" t="s" s="7">
         <v>62</v>
       </c>
-      <c r="D27" t="s" s="6">
+      <c r="D27" t="s" s="7">
         <v>63</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" t="s" s="6">
+      <c r="A28" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" t="s" s="9">
+      <c r="A30" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B30" t="s" s="10">
+      <c r="B30" t="s" s="15">
         <v>64</v>
       </c>
-      <c r="C30" t="s" s="10">
+      <c r="C30" t="s" s="15">
         <v>65</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
     </row>
     <row r="31" ht="15" customHeight="1">
-      <c r="A31" t="s" s="13">
+      <c r="A31" t="s" s="18">
         <v>66</v>
       </c>
-      <c r="B31" t="s" s="13">
+      <c r="B31" t="s" s="18">
         <v>67</v>
       </c>
-      <c r="C31" t="s" s="13">
+      <c r="C31" t="s" s="18">
         <v>68</v>
       </c>
-      <c r="D31" t="s" s="13">
+      <c r="D31" t="s" s="18">
         <v>69</v>
       </c>
-      <c r="E31" s="14"/>
+      <c r="E31" s="19"/>
     </row>
     <row r="32" ht="15" customHeight="1">
-      <c r="A32" t="s" s="6">
+      <c r="A32" t="s" s="7">
         <v>70</v>
       </c>
-      <c r="B32" t="s" s="6">
+      <c r="B32" t="s" s="7">
         <v>71</v>
       </c>
-      <c r="C32" t="s" s="6">
+      <c r="C32" t="s" s="7">
         <v>72</v>
       </c>
-      <c r="D32" t="s" s="6">
+      <c r="D32" t="s" s="7">
         <v>73</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="11"/>
     </row>
     <row r="33" ht="15" customHeight="1">
-      <c r="A33" t="s" s="6">
+      <c r="A33" t="s" s="7">
         <v>74</v>
       </c>
-      <c r="B33" t="s" s="6">
+      <c r="B33" t="s" s="7">
         <v>75</v>
       </c>
-      <c r="C33" t="s" s="6">
+      <c r="C33" t="s" s="7">
         <v>76</v>
       </c>
-      <c r="D33" t="s" s="6">
+      <c r="D33" t="s" s="7">
         <v>77</v>
       </c>
-      <c r="E33" s="7"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" ht="15" customHeight="1">
-      <c r="A34" t="s" s="6">
+      <c r="A34" t="s" s="7">
         <v>78</v>
       </c>
-      <c r="B34" t="s" s="6">
+      <c r="B34" t="s" s="7">
         <v>79</v>
       </c>
-      <c r="C34" t="s" s="6">
+      <c r="C34" t="s" s="7">
         <v>80</v>
       </c>
-      <c r="D34" t="s" s="6">
+      <c r="D34" t="s" s="7">
         <v>81</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="11"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" t="s" s="6">
+      <c r="A35" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" t="s" s="9">
+      <c r="A37" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B37" t="s" s="10">
+      <c r="B37" t="s" s="15">
         <v>82</v>
       </c>
-      <c r="C37" t="s" s="10">
+      <c r="C37" t="s" s="15">
         <v>83</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="12"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="17"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" t="s" s="15">
+      <c r="A38" t="s" s="21">
         <v>84</v>
       </c>
-      <c r="B38" t="s" s="15">
+      <c r="B38" t="s" s="21">
         <v>85</v>
       </c>
-      <c r="C38" t="s" s="15">
+      <c r="C38" t="s" s="21">
         <v>86</v>
       </c>
-      <c r="D38" t="s" s="15">
+      <c r="D38" t="s" s="21">
         <v>87</v>
       </c>
-      <c r="E38" t="s" s="15">
+      <c r="E38" t="s" s="21">
         <v>88</v>
       </c>
     </row>
@@ -2272,242 +2379,242 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.3333" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="16" customWidth="1"/>
-    <col min="2" max="2" width="10" style="16" customWidth="1"/>
-    <col min="3" max="3" width="19.6719" style="16" customWidth="1"/>
-    <col min="4" max="4" width="17.3516" style="16" customWidth="1"/>
-    <col min="5" max="5" width="17.3516" style="16" customWidth="1"/>
-    <col min="6" max="256" width="17.3516" style="16" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="22" customWidth="1"/>
+    <col min="2" max="2" width="10" style="22" customWidth="1"/>
+    <col min="3" max="3" width="19.6719" style="22" customWidth="1"/>
+    <col min="4" max="4" width="17.3516" style="22" customWidth="1"/>
+    <col min="5" max="5" width="17.3516" style="22" customWidth="1"/>
+    <col min="6" max="256" width="17.3516" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="17">
+      <c r="A1" t="s" s="23">
         <v>93</v>
       </c>
-      <c r="B1" t="s" s="17">
+      <c r="B1" t="s" s="23">
         <v>3</v>
       </c>
-      <c r="C1" t="s" s="17">
+      <c r="C1" t="s" s="23">
         <v>4</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" t="s" s="19">
+      <c r="A3" t="s" s="25">
         <v>94</v>
       </c>
-      <c r="B3" t="s" s="19">
+      <c r="B3" t="s" s="25">
         <v>95</v>
       </c>
-      <c r="C3" t="s" s="19">
+      <c r="C3" t="s" s="25">
         <v>96</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" t="s" s="19">
+      <c r="A4" t="s" s="25">
         <v>94</v>
       </c>
-      <c r="B4" t="s" s="19">
+      <c r="B4" t="s" s="25">
         <v>97</v>
       </c>
-      <c r="C4" t="s" s="19">
+      <c r="C4" t="s" s="25">
         <v>98</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" t="s" s="19">
+      <c r="A5" t="s" s="25">
         <v>94</v>
       </c>
-      <c r="B5" t="s" s="19">
+      <c r="B5" t="s" s="25">
         <v>99</v>
       </c>
-      <c r="C5" t="s" s="19">
+      <c r="C5" t="s" s="25">
         <v>100</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" t="s" s="19">
+      <c r="A6" t="s" s="25">
         <v>94</v>
       </c>
-      <c r="B6" t="s" s="19">
+      <c r="B6" t="s" s="25">
         <v>101</v>
       </c>
-      <c r="C6" t="s" s="19">
+      <c r="C6" t="s" s="25">
         <v>102</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" t="s" s="19">
+      <c r="A8" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="24">
         <v>1</v>
       </c>
-      <c r="C8" t="s" s="19">
+      <c r="C8" t="s" s="25">
         <v>104</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" t="s" s="19">
+      <c r="A9" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="24">
         <v>2</v>
       </c>
-      <c r="C9" t="s" s="19">
+      <c r="C9" t="s" s="25">
         <v>105</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" t="s" s="19">
+      <c r="A10" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="24">
         <v>3</v>
       </c>
-      <c r="C10" t="s" s="19">
+      <c r="C10" t="s" s="25">
         <v>106</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" t="s" s="19">
+      <c r="A11" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="24">
         <v>4</v>
       </c>
-      <c r="C11" t="s" s="19">
+      <c r="C11" t="s" s="25">
         <v>107</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" t="s" s="19">
+      <c r="A12" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="24">
         <v>5</v>
       </c>
-      <c r="C12" t="s" s="19">
+      <c r="C12" t="s" s="25">
         <v>108</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" t="s" s="19">
+      <c r="A13" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="24">
         <v>6</v>
       </c>
-      <c r="C13" t="s" s="19">
+      <c r="C13" t="s" s="25">
         <v>109</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" t="s" s="19">
+      <c r="A14" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="24">
         <v>7</v>
       </c>
-      <c r="C14" t="s" s="19">
+      <c r="C14" t="s" s="25">
         <v>110</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" t="s" s="19">
+      <c r="A15" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="24">
         <v>8</v>
       </c>
-      <c r="C15" t="s" s="19">
+      <c r="C15" t="s" s="25">
         <v>111</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="19">
+      <c r="A17" t="s" s="25">
         <v>44</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="24">
         <v>1</v>
       </c>
-      <c r="C17" t="s" s="19">
+      <c r="C17" t="s" s="25">
         <v>104</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
@@ -2531,12 +2638,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.3333" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17.1719" style="20" customWidth="1"/>
-    <col min="2" max="2" width="17.1719" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.1719" style="20" customWidth="1"/>
-    <col min="4" max="4" width="17.1719" style="20" customWidth="1"/>
-    <col min="5" max="5" width="17.1719" style="20" customWidth="1"/>
-    <col min="6" max="256" width="17.3516" style="20" customWidth="1"/>
+    <col min="1" max="1" width="17.1719" style="26" customWidth="1"/>
+    <col min="2" max="2" width="17.1719" style="26" customWidth="1"/>
+    <col min="3" max="3" width="17.1719" style="26" customWidth="1"/>
+    <col min="4" max="4" width="17.1719" style="26" customWidth="1"/>
+    <col min="5" max="5" width="17.1719" style="26" customWidth="1"/>
+    <col min="6" max="256" width="17.3516" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2546,90 +2653,90 @@
       <c r="B1" t="s" s="5">
         <v>113</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="7">
         <v>114</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" t="s" s="7">
         <v>115</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Updated questionnaire model to allow for 2500 character labels (#661)
</commit_message>
<xml_diff>
--- a/cadasta/questionnaires/tests/files/xls-form.xlsx
+++ b/cadasta/questionnaires/tests/files/xls-form.xlsx
@@ -43,8 +43,19 @@
     <t>intro</t>
   </si>
   <si>
-    <t>This form showcases the different question types available in XLSForm. 
-The hints explain how these question types were created.</t>
+    <t>Este formulário é utilizado para capturar informação sobre os encontros com a comunidade durante o processo de delimitação.
+Estes encontros podem ser com a comunidade em geral, com a liderança, ou com povoados dentro da comunidade.  Podiam ser também seminários ao nível do posto administrativo ou distrito.
+O formulário devia ser preenchido cada vez que haja um encontro.
+Os encontros podem envolver actividades de:
+- divulgação das legislações
+- palestras, sessões de vídeo, etc.
+- sensibilização sobre o processo de delimitação da área comunitária
+- sensibilização sobre a criação da associação comunitária
+- escolha de representantes da associação 
+- encontros no ambito do DRP (historial da comunidade, organização social, etc)
+- encontros para confirmar os limites ou encontros de devolução
+O técnico pode usar o formulário para gravar informação sobre a data e lugar do encontro, o numero de participantes e os temas abordados.  Pode também gravar nomes e detalhes pessoais de representantes.
+Por favor deslizar para a frente para continuar.</t>
   </si>
   <si>
     <t>begin group</t>
@@ -372,7 +383,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -393,6 +404,11 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="4">
@@ -415,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -447,6 +463,79 @@
       </right>
       <top style="thin">
         <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -495,7 +584,7 @@
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
@@ -514,34 +603,52 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1769,7 +1876,7 @@
       <c r="B1" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="C1" t="s" s="5">
+      <c r="C1" t="s" s="6">
         <v>4</v>
       </c>
       <c r="D1" t="s" s="5">
@@ -1780,451 +1887,451 @@
       </c>
     </row>
     <row r="2" ht="27" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" t="s" s="9">
         <v>9</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" t="s" s="9">
+      <c r="A4" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="10">
+      <c r="B4" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C4" t="s" s="15">
         <v>12</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" t="s" s="13">
+      <c r="A5" t="s" s="18">
         <v>13</v>
       </c>
-      <c r="B5" t="s" s="13">
+      <c r="B5" t="s" s="18">
         <v>14</v>
       </c>
-      <c r="C5" t="s" s="13">
+      <c r="C5" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="D5" t="s" s="13">
+      <c r="D5" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" t="s" s="6">
+      <c r="A6" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" ht="8.25" customHeight="1">
-      <c r="A8" t="s" s="9">
+      <c r="A8" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B8" t="s" s="10">
+      <c r="B8" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="C8" t="s" s="10">
+      <c r="C8" t="s" s="15">
         <v>19</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" ht="51" customHeight="1">
-      <c r="A9" t="s" s="13">
+      <c r="A9" t="s" s="18">
         <v>20</v>
       </c>
-      <c r="B9" t="s" s="13">
+      <c r="B9" t="s" s="18">
         <v>21</v>
       </c>
-      <c r="C9" t="s" s="13">
+      <c r="C9" t="s" s="18">
         <v>22</v>
       </c>
-      <c r="D9" t="s" s="13">
+      <c r="D9" t="s" s="18">
         <v>23</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
-      <c r="A10" t="s" s="6">
+      <c r="A10" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="B10" t="s" s="6">
+      <c r="B10" t="s" s="7">
         <v>25</v>
       </c>
-      <c r="C10" t="s" s="6">
+      <c r="C10" t="s" s="7">
         <v>26</v>
       </c>
-      <c r="D10" t="s" s="6">
+      <c r="D10" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" ht="16.5" customHeight="1">
-      <c r="A11" t="s" s="6">
+      <c r="A11" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" ht="16.5" customHeight="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" t="s" s="9">
+      <c r="A13" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B13" t="s" s="10">
+      <c r="B13" t="s" s="15">
         <v>28</v>
       </c>
-      <c r="C13" t="s" s="10">
+      <c r="C13" t="s" s="15">
         <v>29</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" ht="51" customHeight="1">
-      <c r="A14" t="s" s="13">
+      <c r="A14" t="s" s="18">
         <v>30</v>
       </c>
-      <c r="B14" t="s" s="13">
+      <c r="B14" t="s" s="18">
         <v>31</v>
       </c>
-      <c r="C14" t="s" s="13">
+      <c r="C14" t="s" s="18">
         <v>32</v>
       </c>
-      <c r="D14" t="s" s="13">
+      <c r="D14" t="s" s="18">
         <v>33</v>
       </c>
-      <c r="E14" s="14"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" t="s" s="6">
+      <c r="A15" t="s" s="7">
         <v>34</v>
       </c>
-      <c r="B15" t="s" s="6">
+      <c r="B15" t="s" s="7">
         <v>35</v>
       </c>
-      <c r="C15" t="s" s="6">
+      <c r="C15" t="s" s="7">
         <v>36</v>
       </c>
-      <c r="D15" t="s" s="6">
+      <c r="D15" t="s" s="7">
         <v>37</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" ht="25.5" customHeight="1">
-      <c r="A16" t="s" s="6">
+      <c r="A16" t="s" s="7">
         <v>38</v>
       </c>
-      <c r="B16" t="s" s="6">
+      <c r="B16" t="s" s="7">
         <v>38</v>
       </c>
-      <c r="C16" t="s" s="6">
+      <c r="C16" t="s" s="7">
         <v>39</v>
       </c>
-      <c r="D16" t="s" s="6">
+      <c r="D16" t="s" s="7">
         <v>40</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="6">
+      <c r="A17" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" t="s" s="9">
+      <c r="A19" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B19" t="s" s="10">
+      <c r="B19" t="s" s="15">
         <v>41</v>
       </c>
-      <c r="C19" t="s" s="10">
+      <c r="C19" t="s" s="15">
         <v>42</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" ht="76.5" customHeight="1">
-      <c r="A20" t="s" s="13">
+      <c r="A20" t="s" s="18">
         <v>43</v>
       </c>
-      <c r="B20" t="s" s="13">
+      <c r="B20" t="s" s="18">
         <v>44</v>
       </c>
-      <c r="C20" t="s" s="13">
+      <c r="C20" t="s" s="18">
         <v>45</v>
       </c>
-      <c r="D20" t="s" s="13">
+      <c r="D20" t="s" s="18">
         <v>46</v>
       </c>
-      <c r="E20" s="14"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" ht="25.5" customHeight="1">
-      <c r="A21" t="s" s="6">
+      <c r="A21" t="s" s="7">
         <v>47</v>
       </c>
-      <c r="B21" t="s" s="6">
+      <c r="B21" t="s" s="7">
         <v>48</v>
       </c>
-      <c r="C21" t="s" s="6">
+      <c r="C21" t="s" s="7">
         <v>49</v>
       </c>
-      <c r="D21" t="s" s="6">
+      <c r="D21" t="s" s="7">
         <v>50</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" t="s" s="6">
+      <c r="A22" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
     </row>
     <row r="24" ht="15" customHeight="1">
-      <c r="A24" t="s" s="9">
+      <c r="A24" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B24" t="s" s="10">
+      <c r="B24" t="s" s="15">
         <v>51</v>
       </c>
-      <c r="C24" t="s" s="10">
+      <c r="C24" t="s" s="15">
         <v>52</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" ht="15" customHeight="1">
-      <c r="A25" t="s" s="13">
+      <c r="A25" t="s" s="18">
         <v>51</v>
       </c>
-      <c r="B25" t="s" s="13">
+      <c r="B25" t="s" s="18">
         <v>53</v>
       </c>
-      <c r="C25" t="s" s="13">
+      <c r="C25" t="s" s="18">
         <v>54</v>
       </c>
-      <c r="D25" t="s" s="13">
+      <c r="D25" t="s" s="18">
         <v>55</v>
       </c>
-      <c r="E25" s="14"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" t="s" s="6">
+      <c r="A26" t="s" s="7">
         <v>56</v>
       </c>
-      <c r="B26" t="s" s="6">
+      <c r="B26" t="s" s="7">
         <v>57</v>
       </c>
-      <c r="C26" t="s" s="6">
+      <c r="C26" t="s" s="7">
         <v>58</v>
       </c>
-      <c r="D26" t="s" s="6">
+      <c r="D26" t="s" s="7">
         <v>59</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" t="s" s="6">
+      <c r="A27" t="s" s="7">
         <v>60</v>
       </c>
-      <c r="B27" t="s" s="6">
+      <c r="B27" t="s" s="7">
         <v>61</v>
       </c>
-      <c r="C27" t="s" s="6">
+      <c r="C27" t="s" s="7">
         <v>62</v>
       </c>
-      <c r="D27" t="s" s="6">
+      <c r="D27" t="s" s="7">
         <v>63</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" t="s" s="6">
+      <c r="A28" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" t="s" s="9">
+      <c r="A30" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B30" t="s" s="10">
+      <c r="B30" t="s" s="15">
         <v>64</v>
       </c>
-      <c r="C30" t="s" s="10">
+      <c r="C30" t="s" s="15">
         <v>65</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
     </row>
     <row r="31" ht="15" customHeight="1">
-      <c r="A31" t="s" s="13">
+      <c r="A31" t="s" s="18">
         <v>66</v>
       </c>
-      <c r="B31" t="s" s="13">
+      <c r="B31" t="s" s="18">
         <v>67</v>
       </c>
-      <c r="C31" t="s" s="13">
+      <c r="C31" t="s" s="18">
         <v>68</v>
       </c>
-      <c r="D31" t="s" s="13">
+      <c r="D31" t="s" s="18">
         <v>69</v>
       </c>
-      <c r="E31" s="14"/>
+      <c r="E31" s="19"/>
     </row>
     <row r="32" ht="15" customHeight="1">
-      <c r="A32" t="s" s="6">
+      <c r="A32" t="s" s="7">
         <v>70</v>
       </c>
-      <c r="B32" t="s" s="6">
+      <c r="B32" t="s" s="7">
         <v>71</v>
       </c>
-      <c r="C32" t="s" s="6">
+      <c r="C32" t="s" s="7">
         <v>72</v>
       </c>
-      <c r="D32" t="s" s="6">
+      <c r="D32" t="s" s="7">
         <v>73</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="11"/>
     </row>
     <row r="33" ht="15" customHeight="1">
-      <c r="A33" t="s" s="6">
+      <c r="A33" t="s" s="7">
         <v>74</v>
       </c>
-      <c r="B33" t="s" s="6">
+      <c r="B33" t="s" s="7">
         <v>75</v>
       </c>
-      <c r="C33" t="s" s="6">
+      <c r="C33" t="s" s="7">
         <v>76</v>
       </c>
-      <c r="D33" t="s" s="6">
+      <c r="D33" t="s" s="7">
         <v>77</v>
       </c>
-      <c r="E33" s="7"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" ht="15" customHeight="1">
-      <c r="A34" t="s" s="6">
+      <c r="A34" t="s" s="7">
         <v>78</v>
       </c>
-      <c r="B34" t="s" s="6">
+      <c r="B34" t="s" s="7">
         <v>79</v>
       </c>
-      <c r="C34" t="s" s="6">
+      <c r="C34" t="s" s="7">
         <v>80</v>
       </c>
-      <c r="D34" t="s" s="6">
+      <c r="D34" t="s" s="7">
         <v>81</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="11"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" t="s" s="6">
+      <c r="A35" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" t="s" s="9">
+      <c r="A37" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="B37" t="s" s="10">
+      <c r="B37" t="s" s="15">
         <v>82</v>
       </c>
-      <c r="C37" t="s" s="10">
+      <c r="C37" t="s" s="15">
         <v>83</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="12"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="17"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" t="s" s="15">
+      <c r="A38" t="s" s="21">
         <v>84</v>
       </c>
-      <c r="B38" t="s" s="15">
+      <c r="B38" t="s" s="21">
         <v>85</v>
       </c>
-      <c r="C38" t="s" s="15">
+      <c r="C38" t="s" s="21">
         <v>86</v>
       </c>
-      <c r="D38" t="s" s="15">
+      <c r="D38" t="s" s="21">
         <v>87</v>
       </c>
-      <c r="E38" t="s" s="15">
+      <c r="E38" t="s" s="21">
         <v>88</v>
       </c>
     </row>
@@ -2272,242 +2379,242 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.3333" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="16" customWidth="1"/>
-    <col min="2" max="2" width="10" style="16" customWidth="1"/>
-    <col min="3" max="3" width="19.6719" style="16" customWidth="1"/>
-    <col min="4" max="4" width="17.3516" style="16" customWidth="1"/>
-    <col min="5" max="5" width="17.3516" style="16" customWidth="1"/>
-    <col min="6" max="256" width="17.3516" style="16" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="22" customWidth="1"/>
+    <col min="2" max="2" width="10" style="22" customWidth="1"/>
+    <col min="3" max="3" width="19.6719" style="22" customWidth="1"/>
+    <col min="4" max="4" width="17.3516" style="22" customWidth="1"/>
+    <col min="5" max="5" width="17.3516" style="22" customWidth="1"/>
+    <col min="6" max="256" width="17.3516" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="17">
+      <c r="A1" t="s" s="23">
         <v>93</v>
       </c>
-      <c r="B1" t="s" s="17">
+      <c r="B1" t="s" s="23">
         <v>3</v>
       </c>
-      <c r="C1" t="s" s="17">
+      <c r="C1" t="s" s="23">
         <v>4</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" t="s" s="19">
+      <c r="A3" t="s" s="25">
         <v>94</v>
       </c>
-      <c r="B3" t="s" s="19">
+      <c r="B3" t="s" s="25">
         <v>95</v>
       </c>
-      <c r="C3" t="s" s="19">
+      <c r="C3" t="s" s="25">
         <v>96</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" t="s" s="19">
+      <c r="A4" t="s" s="25">
         <v>94</v>
       </c>
-      <c r="B4" t="s" s="19">
+      <c r="B4" t="s" s="25">
         <v>97</v>
       </c>
-      <c r="C4" t="s" s="19">
+      <c r="C4" t="s" s="25">
         <v>98</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" t="s" s="19">
+      <c r="A5" t="s" s="25">
         <v>94</v>
       </c>
-      <c r="B5" t="s" s="19">
+      <c r="B5" t="s" s="25">
         <v>99</v>
       </c>
-      <c r="C5" t="s" s="19">
+      <c r="C5" t="s" s="25">
         <v>100</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" t="s" s="19">
+      <c r="A6" t="s" s="25">
         <v>94</v>
       </c>
-      <c r="B6" t="s" s="19">
+      <c r="B6" t="s" s="25">
         <v>101</v>
       </c>
-      <c r="C6" t="s" s="19">
+      <c r="C6" t="s" s="25">
         <v>102</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" t="s" s="19">
+      <c r="A8" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="24">
         <v>1</v>
       </c>
-      <c r="C8" t="s" s="19">
+      <c r="C8" t="s" s="25">
         <v>104</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" t="s" s="19">
+      <c r="A9" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="24">
         <v>2</v>
       </c>
-      <c r="C9" t="s" s="19">
+      <c r="C9" t="s" s="25">
         <v>105</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" t="s" s="19">
+      <c r="A10" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="24">
         <v>3</v>
       </c>
-      <c r="C10" t="s" s="19">
+      <c r="C10" t="s" s="25">
         <v>106</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" t="s" s="19">
+      <c r="A11" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="24">
         <v>4</v>
       </c>
-      <c r="C11" t="s" s="19">
+      <c r="C11" t="s" s="25">
         <v>107</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" t="s" s="19">
+      <c r="A12" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="24">
         <v>5</v>
       </c>
-      <c r="C12" t="s" s="19">
+      <c r="C12" t="s" s="25">
         <v>108</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" t="s" s="19">
+      <c r="A13" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="24">
         <v>6</v>
       </c>
-      <c r="C13" t="s" s="19">
+      <c r="C13" t="s" s="25">
         <v>109</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" t="s" s="19">
+      <c r="A14" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="24">
         <v>7</v>
       </c>
-      <c r="C14" t="s" s="19">
+      <c r="C14" t="s" s="25">
         <v>110</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" t="s" s="19">
+      <c r="A15" t="s" s="25">
         <v>103</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="24">
         <v>8</v>
       </c>
-      <c r="C15" t="s" s="19">
+      <c r="C15" t="s" s="25">
         <v>111</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" t="s" s="19">
+      <c r="A17" t="s" s="25">
         <v>44</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="24">
         <v>1</v>
       </c>
-      <c r="C17" t="s" s="19">
+      <c r="C17" t="s" s="25">
         <v>104</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
@@ -2531,12 +2638,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.3333" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17.1719" style="20" customWidth="1"/>
-    <col min="2" max="2" width="17.1719" style="20" customWidth="1"/>
-    <col min="3" max="3" width="17.1719" style="20" customWidth="1"/>
-    <col min="4" max="4" width="17.1719" style="20" customWidth="1"/>
-    <col min="5" max="5" width="17.1719" style="20" customWidth="1"/>
-    <col min="6" max="256" width="17.3516" style="20" customWidth="1"/>
+    <col min="1" max="1" width="17.1719" style="26" customWidth="1"/>
+    <col min="2" max="2" width="17.1719" style="26" customWidth="1"/>
+    <col min="3" max="3" width="17.1719" style="26" customWidth="1"/>
+    <col min="4" max="4" width="17.1719" style="26" customWidth="1"/>
+    <col min="5" max="5" width="17.1719" style="26" customWidth="1"/>
+    <col min="6" max="256" width="17.3516" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2546,90 +2653,90 @@
       <c r="B1" t="s" s="5">
         <v>113</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="7">
         <v>114</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" t="s" s="7">
         <v>115</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>